<commit_message>
Committing code with test data changes, new test cases of Drop 3 etc.
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/DeleteCustomFilter.xlsx
+++ b/BloodstreamAPI/testData/DeleteCustomFilter.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C12DD0E-50FF-47BE-9A6F-EE18FE6D7897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A65A93-ECBA-490E-BC49-ACDFD4EDFFFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="715" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DelConclToApprove" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="19">
   <si>
     <t>EndPoint</t>
   </si>
@@ -60,12 +60,34 @@
   </si>
   <si>
     <t>WorklistInformation</t>
+  </si>
+  <si>
+    <t>ConclusionsToApprovert</t>
+  </si>
+  <si>
+    <t>DonationInformationry</t>
+  </si>
+  <si>
+    <t>TestInformationrty</t>
+  </si>
+  <si>
+    <t>WorklistConclusionsyrt</t>
+  </si>
+  <si>
+    <t>WorklistInformationty</t>
+  </si>
+  <si>
+    <t>124$</t>
+  </si>
+  <si>
+    <t>123$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,17 +450,17 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="26.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="8.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="15.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="14.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -466,7 +488,9 @@
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -515,7 +539,7 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
@@ -526,12 +550,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C12" s="6"/>
     </row>
@@ -550,16 +574,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA324F4-6303-45A9-B72B-667907D5EA0F}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -587,7 +611,9 @@
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -649,12 +675,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C12" s="6"/>
     </row>
@@ -673,12 +699,12 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -706,7 +732,9 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -773,7 +801,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C12" s="6"/>
     </row>
@@ -792,12 +820,12 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C12"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" customWidth="true" width="18.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -825,7 +853,9 @@
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -892,7 +922,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C12" s="6"/>
     </row>
@@ -910,14 +940,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6AE23C-ED38-43E1-8869-59A543319E62}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -945,7 +975,9 @@
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -1012,7 +1044,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C12" s="6"/>
     </row>

</xml_diff>

<commit_message>
optimized code, added extra test cases-Drop 1 to Drop 3
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/DeleteCustomFilter.xlsx
+++ b/BloodstreamAPI/testData/DeleteCustomFilter.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="24">
   <si>
     <t>EndPoint</t>
   </si>
@@ -81,6 +81,21 @@
   </si>
   <si>
     <t>123$</t>
+  </si>
+  <si>
+    <t>456$</t>
+  </si>
+  <si>
+    <t>786$</t>
+  </si>
+  <si>
+    <t>900$</t>
+  </si>
+  <si>
+    <t>880$</t>
+  </si>
+  <si>
+    <t>678$</t>
   </si>
 </sst>
 </file>
@@ -489,7 +504,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -612,7 +627,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -733,7 +748,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -854,7 +869,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -976,7 +991,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>